<commit_message>
Add correct model name to the regions sheet.
</commit_message>
<xml_diff>
--- a/ar6/registration_templates/IPCC_AR6_model_registration_REMIND_2.1-MAgPIE_4.2.xlsx
+++ b/ar6/registration_templates/IPCC_AR6_model_registration_REMIND_2.1-MAgPIE_4.2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -3330,76 +3330,76 @@
     <t xml:space="preserve">Native Region Name (for explanatory purposes, &lt; 128 characters)</t>
   </si>
   <si>
+    <t xml:space="preserve">CHA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">China</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EU 28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">India</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Japan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Latin America and the Caribbean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Middle East, North Africa, Central Asia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sub-saharan Africa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">United States of America</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">other Asia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canada, NZ, Australia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-EU28 Europe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Region Mapping for standardized regions (World, 5 SSP regions, large emitting countries/regions)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Native Region Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standardized Region Code</t>
+  </si>
+  <si>
     <t xml:space="preserve">REMIND-EDGET 2.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">China</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EUR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EU 28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">India</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Japan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LAM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Latin America and the Caribbean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MEA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Middle East, North Africa, Central Asia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SSA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sub-saharan Africa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">United States of America</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">other Asia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Canada, NZ, Australia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NEU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-EU28 Europe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Region Mapping for standardized regions (World, 5 SSP regions, large emitting countries/regions)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Native Region Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Standardized Region Code</t>
   </si>
   <si>
     <t xml:space="preserve">Native Region Name</t>
@@ -4105,7 +4105,7 @@
   <dimension ref="A1:N316"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
+      <selection pane="topLeft" activeCell="A29" activeCellId="1" sqref="A3:A13 A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7114,7 +7114,7 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="1" sqref="A3:A13 C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7491,8 +7491,8 @@
   </sheetPr>
   <dimension ref="A1:MQ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AM1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AQ10" activeCellId="0" sqref="AQ10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AM1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AQ10" activeCellId="1" sqref="A3:A13 AQ10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11741,13 +11741,13 @@
   </sheetPr>
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="68" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="68" width="23.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="69" width="19.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="69" width="59.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="9.13"/>
@@ -11766,76 +11766,76 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="68" t="s">
+        <v>589</v>
+      </c>
+      <c r="B2" s="69" t="s">
         <v>1006</v>
       </c>
-      <c r="B2" s="69" t="s">
+      <c r="C2" s="69" t="s">
         <v>1007</v>
-      </c>
-      <c r="C2" s="69" t="s">
-        <v>1008</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="68" t="s">
-        <v>1006</v>
+        <v>589</v>
       </c>
       <c r="B3" s="69" t="s">
+        <v>1008</v>
+      </c>
+      <c r="C3" s="69" t="s">
         <v>1009</v>
-      </c>
-      <c r="C3" s="69" t="s">
-        <v>1010</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="68" t="s">
-        <v>1006</v>
+        <v>589</v>
       </c>
       <c r="B4" s="69" t="s">
         <v>288</v>
       </c>
       <c r="C4" s="69" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="68" t="s">
-        <v>1006</v>
+        <v>589</v>
       </c>
       <c r="B5" s="69" t="s">
         <v>310</v>
       </c>
       <c r="C5" s="69" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="68" t="s">
-        <v>1006</v>
+        <v>589</v>
       </c>
       <c r="B6" s="69" t="s">
+        <v>1012</v>
+      </c>
+      <c r="C6" s="69" t="s">
         <v>1013</v>
-      </c>
-      <c r="C6" s="69" t="s">
-        <v>1014</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="68" t="s">
-        <v>1006</v>
+        <v>589</v>
       </c>
       <c r="B7" s="69" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C7" s="69" t="s">
         <v>1015</v>
-      </c>
-      <c r="C7" s="69" t="s">
-        <v>1016</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="68" t="s">
-        <v>1006</v>
+        <v>589</v>
       </c>
       <c r="B8" s="69" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="C8" s="69" t="s">
         <v>33</v>
@@ -11843,57 +11843,57 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="68" t="s">
-        <v>1006</v>
+        <v>589</v>
       </c>
       <c r="B9" s="69" t="s">
+        <v>1017</v>
+      </c>
+      <c r="C9" s="69" t="s">
         <v>1018</v>
-      </c>
-      <c r="C9" s="69" t="s">
-        <v>1019</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="68" t="s">
-        <v>1006</v>
+        <v>589</v>
       </c>
       <c r="B10" s="69" t="s">
         <v>546</v>
       </c>
       <c r="C10" s="69" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="68" t="s">
-        <v>1006</v>
+        <v>589</v>
       </c>
       <c r="B11" s="69" t="s">
+        <v>1020</v>
+      </c>
+      <c r="C11" s="69" t="s">
         <v>1021</v>
-      </c>
-      <c r="C11" s="69" t="s">
-        <v>1022</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="68" t="s">
-        <v>1006</v>
+        <v>589</v>
       </c>
       <c r="B12" s="69" t="s">
+        <v>1022</v>
+      </c>
+      <c r="C12" s="69" t="s">
         <v>1023</v>
-      </c>
-      <c r="C12" s="69" t="s">
-        <v>1024</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="68" t="s">
-        <v>1006</v>
+        <v>589</v>
       </c>
       <c r="B13" s="69" t="s">
+        <v>1024</v>
+      </c>
+      <c r="C13" s="69" t="s">
         <v>1025</v>
-      </c>
-      <c r="C13" s="69" t="s">
-        <v>1026</v>
       </c>
     </row>
   </sheetData>
@@ -11916,7 +11916,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="1" sqref="A3:A13 B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11929,7 +11929,7 @@
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="73" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="B1" s="73"/>
       <c r="C1" s="73"/>
@@ -11939,18 +11939,18 @@
         <v>581</v>
       </c>
       <c r="B2" s="74" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C2" s="75" t="s">
         <v>1028</v>
-      </c>
-      <c r="C2" s="75" t="s">
-        <v>1029</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="68" t="s">
-        <v>1006</v>
+        <v>1029</v>
       </c>
       <c r="B3" s="69" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="C3" s="72" t="s">
         <v>38</v>
@@ -11958,10 +11958,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="68" t="s">
-        <v>1006</v>
+        <v>1029</v>
       </c>
       <c r="B4" s="69" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="C4" s="72" t="s">
         <v>38</v>
@@ -11969,10 +11969,10 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="68" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B5" s="69" t="s">
         <v>1006</v>
-      </c>
-      <c r="B5" s="69" t="s">
-        <v>1007</v>
       </c>
       <c r="C5" s="72" t="s">
         <v>35</v>
@@ -11980,7 +11980,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="68" t="s">
-        <v>1006</v>
+        <v>1029</v>
       </c>
       <c r="B6" s="69" t="s">
         <v>288</v>
@@ -11991,10 +11991,10 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="68" t="s">
-        <v>1006</v>
+        <v>1029</v>
       </c>
       <c r="B7" s="69" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="C7" s="72" t="s">
         <v>35</v>
@@ -12002,10 +12002,10 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="68" t="s">
-        <v>1006</v>
+        <v>1029</v>
       </c>
       <c r="B8" s="69" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="C8" s="72" t="s">
         <v>29</v>
@@ -12013,7 +12013,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="68" t="s">
-        <v>1006</v>
+        <v>1029</v>
       </c>
       <c r="B9" s="69" t="s">
         <v>310</v>
@@ -12024,7 +12024,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="68" t="s">
-        <v>1006</v>
+        <v>1029</v>
       </c>
       <c r="B10" s="69" t="s">
         <v>546</v>
@@ -12035,10 +12035,10 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="68" t="s">
-        <v>1006</v>
+        <v>1029</v>
       </c>
       <c r="B11" s="69" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="C11" s="72" t="s">
         <v>29</v>
@@ -12046,10 +12046,10 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="68" t="s">
-        <v>1006</v>
+        <v>1029</v>
       </c>
       <c r="B12" s="69" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="C12" s="72" t="s">
         <v>29</v>
@@ -12057,10 +12057,10 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="68" t="s">
-        <v>1006</v>
+        <v>1029</v>
       </c>
       <c r="B13" s="69" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="C13" s="72" t="s">
         <v>41</v>
@@ -12068,10 +12068,10 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="68" t="s">
-        <v>1006</v>
+        <v>1029</v>
       </c>
       <c r="B14" s="69" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="C14" s="72" t="s">
         <v>32</v>
@@ -12079,7 +12079,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="68" t="s">
-        <v>1006</v>
+        <v>1029</v>
       </c>
       <c r="B15" s="69" t="s">
         <v>546</v>
@@ -12090,10 +12090,10 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="68" t="s">
-        <v>1006</v>
+        <v>1029</v>
       </c>
       <c r="B16" s="69" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="C16" s="72" t="s">
         <v>80</v>
@@ -12101,10 +12101,10 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="68" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B17" s="69" t="s">
         <v>1006</v>
-      </c>
-      <c r="B17" s="69" t="s">
-        <v>1007</v>
       </c>
       <c r="C17" s="72" t="s">
         <v>168</v>
@@ -12112,7 +12112,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="68" t="s">
-        <v>1006</v>
+        <v>1029</v>
       </c>
       <c r="B18" s="69" t="s">
         <v>288</v>
@@ -12123,10 +12123,10 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="68" t="s">
-        <v>1006</v>
+        <v>1029</v>
       </c>
       <c r="B19" s="69" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="C19" s="72" t="s">
         <v>458</v>
@@ -12134,7 +12134,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="68" t="s">
-        <v>1006</v>
+        <v>1029</v>
       </c>
       <c r="B20" s="69" t="s">
         <v>310</v>
@@ -12145,10 +12145,10 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="68" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B21" s="69" t="s">
         <v>1006</v>
-      </c>
-      <c r="B21" s="69" t="s">
-        <v>1007</v>
       </c>
       <c r="C21" s="72" t="s">
         <v>60</v>
@@ -12156,10 +12156,10 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="68" t="s">
-        <v>1006</v>
+        <v>1029</v>
       </c>
       <c r="B22" s="69" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="C22" s="72" t="s">
         <v>52</v>
@@ -12167,7 +12167,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="68" t="s">
-        <v>1006</v>
+        <v>1029</v>
       </c>
       <c r="B23" s="69" t="s">
         <v>288</v>
@@ -12178,7 +12178,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="68" t="s">
-        <v>1006</v>
+        <v>1029</v>
       </c>
       <c r="B24" s="69" t="s">
         <v>310</v>
@@ -12189,10 +12189,10 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="68" t="s">
-        <v>1006</v>
+        <v>1029</v>
       </c>
       <c r="B25" s="69" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="C25" s="72" t="s">
         <v>75</v>
@@ -12200,10 +12200,10 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="68" t="s">
-        <v>1006</v>
+        <v>1029</v>
       </c>
       <c r="B26" s="69" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="C26" s="72" t="s">
         <v>72</v>
@@ -12211,10 +12211,10 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="68" t="s">
-        <v>1006</v>
+        <v>1029</v>
       </c>
       <c r="B27" s="69" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="C27" s="72" t="s">
         <v>58</v>
@@ -12222,10 +12222,10 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="68" t="s">
-        <v>1006</v>
+        <v>1029</v>
       </c>
       <c r="B28" s="69" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="C28" s="72" t="s">
         <v>69</v>
@@ -12233,7 +12233,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="68" t="s">
-        <v>1006</v>
+        <v>1029</v>
       </c>
       <c r="B29" s="69" t="s">
         <v>546</v>
@@ -12244,10 +12244,10 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="68" t="s">
-        <v>1006</v>
+        <v>1029</v>
       </c>
       <c r="B30" s="69" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="C30" s="72" t="s">
         <v>66</v>
@@ -12255,10 +12255,10 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="68" t="s">
-        <v>1006</v>
+        <v>1029</v>
       </c>
       <c r="B31" s="69" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="C31" s="72" t="s">
         <v>77</v>
@@ -12266,10 +12266,10 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="68" t="s">
-        <v>1006</v>
+        <v>1029</v>
       </c>
       <c r="B32" s="69" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="C32" s="72" t="s">
         <v>77</v>
@@ -12297,7 +12297,7 @@
   <dimension ref="A1:J249"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A208" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="L8"/>
+      <selection pane="topLeft" activeCell="L8" activeCellId="1" sqref="A3:A13 L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12325,7 +12325,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B2" s="76"/>
       <c r="C2" s="0" t="s">
@@ -12340,7 +12340,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B3" s="76"/>
       <c r="C3" s="0" t="s">
@@ -12355,7 +12355,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B4" s="76"/>
       <c r="C4" s="0" t="s">
@@ -12370,7 +12370,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B5" s="76"/>
       <c r="C5" s="0" t="s">
@@ -12385,7 +12385,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="76" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B6" s="76"/>
       <c r="C6" s="0" t="s">
@@ -12400,7 +12400,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="76" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B7" s="76"/>
       <c r="C7" s="0" t="s">
@@ -12415,7 +12415,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="76" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B8" s="76"/>
       <c r="C8" s="0" t="s">
@@ -12430,7 +12430,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B9" s="76"/>
       <c r="C9" s="0" t="s">
@@ -12442,7 +12442,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="76" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B10" s="76"/>
       <c r="C10" s="0" t="s">
@@ -12457,7 +12457,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B11" s="76"/>
       <c r="C11" s="0" t="s">
@@ -12472,7 +12472,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="76" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="B12" s="76"/>
       <c r="C12" s="0" t="s">
@@ -12487,7 +12487,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B13" s="76"/>
       <c r="C13" s="0" t="s">
@@ -12502,7 +12502,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B14" s="76"/>
       <c r="C14" s="0" t="s">
@@ -12517,7 +12517,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B15" s="76"/>
       <c r="C15" s="0" t="s">
@@ -12532,7 +12532,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B16" s="76"/>
       <c r="C16" s="0" t="s">
@@ -12547,7 +12547,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="76" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="B17" s="76"/>
       <c r="C17" s="0" t="s">
@@ -12562,7 +12562,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="76" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B18" s="76"/>
       <c r="C18" s="0" t="s">
@@ -12577,7 +12577,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="76" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="B19" s="76"/>
       <c r="C19" s="0" t="s">
@@ -12592,7 +12592,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B20" s="76"/>
       <c r="C20" s="0" t="s">
@@ -12607,7 +12607,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="76" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B21" s="76"/>
       <c r="C21" s="0" t="s">
@@ -12622,7 +12622,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B22" s="76"/>
       <c r="C22" s="0" t="s">
@@ -12637,7 +12637,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B23" s="76"/>
       <c r="C23" s="0" t="s">
@@ -12652,7 +12652,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B24" s="76"/>
       <c r="C24" s="0" t="s">
@@ -12667,7 +12667,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="76" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B25" s="76"/>
       <c r="C25" s="0" t="s">
@@ -12682,7 +12682,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="76" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B26" s="76"/>
       <c r="C26" s="0" t="s">
@@ -12697,7 +12697,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B27" s="76"/>
       <c r="C27" s="0" t="s">
@@ -12712,7 +12712,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="76" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B28" s="76"/>
       <c r="C28" s="0" t="s">
@@ -12727,7 +12727,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B29" s="76"/>
       <c r="C29" s="0" t="s">
@@ -12742,7 +12742,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="76" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="B30" s="76"/>
       <c r="C30" s="0" t="s">
@@ -12757,7 +12757,7 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B31" s="76"/>
       <c r="C31" s="0" t="s">
@@ -12772,7 +12772,7 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B32" s="76"/>
       <c r="C32" s="0" t="s">
@@ -12787,7 +12787,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B33" s="76"/>
       <c r="C33" s="0" t="s">
@@ -12802,7 +12802,7 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B34" s="76"/>
       <c r="C34" s="0" t="s">
@@ -12817,7 +12817,7 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B35" s="76"/>
       <c r="C35" s="0" t="s">
@@ -12832,7 +12832,7 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B36" s="76"/>
       <c r="C36" s="0" t="s">
@@ -12847,7 +12847,7 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B37" s="76"/>
       <c r="C37" s="0" t="s">
@@ -12862,7 +12862,7 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B38" s="76"/>
       <c r="C38" s="0" t="s">
@@ -12877,7 +12877,7 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B39" s="76"/>
       <c r="C39" s="0" t="s">
@@ -12892,7 +12892,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B40" s="76"/>
       <c r="C40" s="0" t="s">
@@ -12907,7 +12907,7 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="76" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="B41" s="76"/>
       <c r="C41" s="0" t="s">
@@ -12922,7 +12922,7 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B42" s="76"/>
       <c r="C42" s="0" t="s">
@@ -12937,7 +12937,7 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="76" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B43" s="76"/>
       <c r="C43" s="0" t="s">
@@ -12952,7 +12952,7 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B44" s="76"/>
       <c r="C44" s="0" t="s">
@@ -12966,7 +12966,7 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="76" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="B45" s="76"/>
       <c r="C45" s="0" t="s">
@@ -12980,7 +12980,7 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B46" s="76"/>
       <c r="C46" s="0" t="s">
@@ -12995,7 +12995,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B47" s="76"/>
       <c r="C47" s="0" t="s">
@@ -13010,7 +13010,7 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B48" s="76"/>
       <c r="C48" s="0" t="s">
@@ -13025,7 +13025,7 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B49" s="76"/>
       <c r="C49" s="0" t="s">
@@ -13040,7 +13040,7 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B50" s="76"/>
       <c r="C50" s="0" t="s">
@@ -13055,7 +13055,7 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B51" s="76"/>
       <c r="C51" s="0" t="s">
@@ -13070,7 +13070,7 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B52" s="76"/>
       <c r="C52" s="0" t="s">
@@ -13085,7 +13085,7 @@
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B53" s="76"/>
       <c r="C53" s="0" t="s">
@@ -13100,7 +13100,7 @@
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B54" s="76"/>
       <c r="C54" s="0" t="s">
@@ -13115,7 +13115,7 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B55" s="76"/>
       <c r="C55" s="0" t="s">
@@ -13130,7 +13130,7 @@
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B56" s="76"/>
       <c r="C56" s="0" t="s">
@@ -13145,7 +13145,7 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B57" s="76"/>
       <c r="C57" s="0" t="s">
@@ -13160,7 +13160,7 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="76" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B58" s="76"/>
       <c r="C58" s="0" t="s">
@@ -13175,7 +13175,7 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="76" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B59" s="76"/>
       <c r="C59" s="0" t="s">
@@ -13190,7 +13190,7 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="76" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B60" s="76"/>
       <c r="C60" s="0" t="s">
@@ -13205,7 +13205,7 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B61" s="76"/>
       <c r="C61" s="0" t="s">
@@ -13220,7 +13220,7 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B62" s="76"/>
       <c r="C62" s="0" t="s">
@@ -13235,7 +13235,7 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="76" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B63" s="76"/>
       <c r="C63" s="0" t="s">
@@ -13250,7 +13250,7 @@
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B64" s="76"/>
       <c r="C64" s="0" t="s">
@@ -13265,7 +13265,7 @@
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="76" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B65" s="76"/>
       <c r="C65" s="0" t="s">
@@ -13280,7 +13280,7 @@
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B66" s="76"/>
       <c r="C66" s="0" t="s">
@@ -13295,7 +13295,7 @@
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="76" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B67" s="76"/>
       <c r="C67" s="0" t="s">
@@ -13310,7 +13310,7 @@
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B68" s="76"/>
       <c r="C68" s="0" t="s">
@@ -13325,7 +13325,7 @@
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="76" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B69" s="76"/>
       <c r="C69" s="0" t="s">
@@ -13340,7 +13340,7 @@
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="76" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B70" s="76"/>
       <c r="C70" s="0" t="s">
@@ -13355,7 +13355,7 @@
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="76" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B71" s="76"/>
       <c r="C71" s="0" t="s">
@@ -13370,7 +13370,7 @@
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B72" s="76"/>
       <c r="C72" s="0" t="s">
@@ -13385,7 +13385,7 @@
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="76" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B73" s="76"/>
       <c r="C73" s="0" t="s">
@@ -13400,7 +13400,7 @@
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B74" s="76"/>
       <c r="C74" s="0" t="s">
@@ -13415,7 +13415,7 @@
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B75" s="76"/>
       <c r="C75" s="0" t="s">
@@ -13430,7 +13430,7 @@
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="76" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B76" s="76"/>
       <c r="C76" s="0" t="s">
@@ -13445,7 +13445,7 @@
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="76" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B77" s="76"/>
       <c r="C77" s="0" t="s">
@@ -13460,7 +13460,7 @@
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B78" s="78"/>
       <c r="C78" s="0" t="s">
@@ -13475,7 +13475,7 @@
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B79" s="76"/>
       <c r="C79" s="0" t="s">
@@ -13490,7 +13490,7 @@
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="76" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B80" s="76"/>
       <c r="C80" s="0" t="s">
@@ -13505,7 +13505,7 @@
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="76" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="B81" s="76"/>
       <c r="C81" s="0" t="s">
@@ -13520,7 +13520,7 @@
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="76" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B82" s="76"/>
       <c r="C82" s="0" t="s">
@@ -13535,7 +13535,7 @@
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B83" s="76"/>
       <c r="C83" s="0" t="s">
@@ -13550,7 +13550,7 @@
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="76" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B84" s="76"/>
       <c r="C84" s="0" t="s">
@@ -13565,7 +13565,7 @@
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B85" s="76"/>
       <c r="C85" s="0" t="s">
@@ -13580,7 +13580,7 @@
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B86" s="76"/>
       <c r="C86" s="0" t="s">
@@ -13595,7 +13595,7 @@
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B87" s="76"/>
       <c r="C87" s="0" t="s">
@@ -13610,7 +13610,7 @@
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B88" s="76"/>
       <c r="C88" s="0" t="s">
@@ -13625,7 +13625,7 @@
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B89" s="78"/>
       <c r="C89" s="0" t="s">
@@ -13640,7 +13640,7 @@
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="76" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B90" s="76"/>
       <c r="C90" s="0" t="s">
@@ -13655,7 +13655,7 @@
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B91" s="76"/>
       <c r="C91" s="0" t="s">
@@ -13670,7 +13670,7 @@
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="76" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B92" s="76"/>
       <c r="C92" s="0" t="s">
@@ -13685,7 +13685,7 @@
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B93" s="76"/>
       <c r="C93" s="0" t="s">
@@ -13700,7 +13700,7 @@
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B94" s="76"/>
       <c r="C94" s="0" t="s">
@@ -13715,7 +13715,7 @@
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B95" s="76"/>
       <c r="C95" s="0" t="s">
@@ -13730,7 +13730,7 @@
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B96" s="76"/>
       <c r="C96" s="0" t="s">
@@ -13745,7 +13745,7 @@
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="76" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="B97" s="76"/>
       <c r="C97" s="0" t="s">
@@ -13760,7 +13760,7 @@
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="76" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="B98" s="76"/>
       <c r="C98" s="0" t="s">
@@ -13775,7 +13775,7 @@
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B99" s="76"/>
       <c r="C99" s="0" t="s">
@@ -13790,7 +13790,7 @@
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="76" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B100" s="76"/>
       <c r="C100" s="0" t="s">
@@ -13805,7 +13805,7 @@
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B101" s="76"/>
       <c r="C101" s="0" t="s">
@@ -13820,7 +13820,7 @@
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="76" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B102" s="76"/>
       <c r="C102" s="0" t="s">
@@ -13835,7 +13835,7 @@
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B103" s="76"/>
       <c r="C103" s="0" t="s">
@@ -13850,7 +13850,7 @@
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="76" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B104" s="76"/>
       <c r="C104" s="0" t="s">
@@ -13880,7 +13880,7 @@
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B106" s="76"/>
       <c r="C106" s="0" t="s">
@@ -13895,7 +13895,7 @@
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="76" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B107" s="76"/>
       <c r="C107" s="0" t="s">
@@ -13910,7 +13910,7 @@
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="76" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B108" s="76"/>
       <c r="C108" s="0" t="s">
@@ -13925,7 +13925,7 @@
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="76" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B109" s="76"/>
       <c r="C109" s="0" t="s">
@@ -13940,7 +13940,7 @@
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="76" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B110" s="76"/>
       <c r="C110" s="0" t="s">
@@ -13955,7 +13955,7 @@
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="76" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B111" s="76"/>
       <c r="C111" s="0" t="s">
@@ -13970,7 +13970,7 @@
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="76" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B112" s="76"/>
       <c r="C112" s="0" t="s">
@@ -13985,7 +13985,7 @@
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B113" s="76"/>
       <c r="C113" s="0" t="s">
@@ -14000,7 +14000,7 @@
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="76" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B114" s="76"/>
       <c r="C114" s="0" t="s">
@@ -14015,7 +14015,7 @@
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="76" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B115" s="76"/>
       <c r="C115" s="0" t="s">
@@ -14045,7 +14045,7 @@
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="76" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="B117" s="76"/>
       <c r="C117" s="0" t="s">
@@ -14060,7 +14060,7 @@
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B118" s="76"/>
       <c r="C118" s="0" t="s">
@@ -14075,7 +14075,7 @@
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="76" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="B119" s="76"/>
       <c r="C119" s="0" t="s">
@@ -14090,7 +14090,7 @@
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B120" s="76"/>
       <c r="C120" s="0" t="s">
@@ -14105,7 +14105,7 @@
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B121" s="76"/>
       <c r="C121" s="0" t="s">
@@ -14120,7 +14120,7 @@
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B122" s="76"/>
       <c r="C122" s="0" t="s">
@@ -14135,7 +14135,7 @@
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B123" s="76"/>
       <c r="C123" s="0" t="s">
@@ -14150,7 +14150,7 @@
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="76" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B124" s="76"/>
       <c r="C124" s="0" t="s">
@@ -14165,7 +14165,7 @@
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B125" s="76"/>
       <c r="C125" s="0" t="s">
@@ -14180,7 +14180,7 @@
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="76" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B126" s="76"/>
       <c r="C126" s="0" t="s">
@@ -14195,7 +14195,7 @@
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B127" s="76"/>
       <c r="C127" s="0" t="s">
@@ -14210,7 +14210,7 @@
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="76" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B128" s="76"/>
       <c r="C128" s="0" t="s">
@@ -14225,7 +14225,7 @@
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B129" s="76"/>
       <c r="C129" s="0" t="s">
@@ -14240,7 +14240,7 @@
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="76" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B130" s="76"/>
       <c r="C130" s="0" t="s">
@@ -14255,7 +14255,7 @@
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B131" s="76"/>
       <c r="C131" s="0" t="s">
@@ -14270,7 +14270,7 @@
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B132" s="76"/>
       <c r="C132" s="0" t="s">
@@ -14285,7 +14285,7 @@
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="76" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B133" s="76"/>
       <c r="C133" s="0" t="s">
@@ -14300,7 +14300,7 @@
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="76" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B134" s="76"/>
       <c r="C134" s="0" t="s">
@@ -14315,7 +14315,7 @@
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="76" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B135" s="76"/>
       <c r="C135" s="0" t="s">
@@ -14330,7 +14330,7 @@
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="76" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="B136" s="76"/>
       <c r="C136" s="0" t="s">
@@ -14345,7 +14345,7 @@
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B137" s="76"/>
       <c r="C137" s="0" t="s">
@@ -14360,7 +14360,7 @@
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="76" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B138" s="76"/>
       <c r="C138" s="0" t="s">
@@ -14375,7 +14375,7 @@
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="76" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B139" s="76"/>
       <c r="C139" s="0" t="s">
@@ -14390,7 +14390,7 @@
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="76" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="B140" s="76"/>
       <c r="C140" s="0" t="s">
@@ -14405,7 +14405,7 @@
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B141" s="76"/>
       <c r="C141" s="0" t="s">
@@ -14420,7 +14420,7 @@
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B142" s="76"/>
       <c r="C142" s="0" t="s">
@@ -14435,7 +14435,7 @@
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B143" s="76"/>
       <c r="C143" s="0" t="s">
@@ -14450,7 +14450,7 @@
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B144" s="76"/>
       <c r="C144" s="0" t="s">
@@ -14465,7 +14465,7 @@
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="76" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B145" s="76"/>
       <c r="C145" s="0" t="s">
@@ -14480,7 +14480,7 @@
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B146" s="76"/>
       <c r="C146" s="0" t="s">
@@ -14495,7 +14495,7 @@
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="76" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B147" s="76"/>
       <c r="C147" s="0" t="s">
@@ -14510,7 +14510,7 @@
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B148" s="76"/>
       <c r="C148" s="0" t="s">
@@ -14525,7 +14525,7 @@
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="76" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B149" s="76"/>
       <c r="C149" s="0" t="s">
@@ -14540,7 +14540,7 @@
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B150" s="76"/>
       <c r="C150" s="0" t="s">
@@ -14555,7 +14555,7 @@
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B151" s="76"/>
       <c r="C151" s="0" t="s">
@@ -14570,7 +14570,7 @@
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B152" s="76"/>
       <c r="C152" s="0" t="s">
@@ -14585,7 +14585,7 @@
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B153" s="76"/>
       <c r="C153" s="0" t="s">
@@ -14600,7 +14600,7 @@
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B154" s="76"/>
       <c r="C154" s="0" t="s">
@@ -14615,7 +14615,7 @@
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B155" s="76"/>
       <c r="C155" s="0" t="s">
@@ -14630,7 +14630,7 @@
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B156" s="76"/>
       <c r="C156" s="0" t="s">
@@ -14645,7 +14645,7 @@
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B157" s="76"/>
       <c r="C157" s="0" t="s">
@@ -14660,7 +14660,7 @@
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B158" s="76"/>
       <c r="C158" s="0" t="s">
@@ -14675,7 +14675,7 @@
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B159" s="76"/>
       <c r="C159" s="0" t="s">
@@ -14690,7 +14690,7 @@
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B160" s="76"/>
       <c r="C160" s="0" t="s">
@@ -14705,7 +14705,7 @@
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B161" s="76"/>
       <c r="C161" s="0" t="s">
@@ -14720,7 +14720,7 @@
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B162" s="76"/>
       <c r="C162" s="0" t="s">
@@ -14735,7 +14735,7 @@
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B163" s="76"/>
       <c r="C163" s="0" t="s">
@@ -14750,7 +14750,7 @@
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B164" s="76"/>
       <c r="C164" s="0" t="s">
@@ -14765,7 +14765,7 @@
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B165" s="76"/>
       <c r="C165" s="0" t="s">
@@ -14780,7 +14780,7 @@
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B166" s="76"/>
       <c r="C166" s="0" t="s">
@@ -14795,7 +14795,7 @@
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="76" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B167" s="76"/>
       <c r="C167" s="0" t="s">
@@ -14810,7 +14810,7 @@
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="76" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B168" s="76"/>
       <c r="C168" s="0" t="s">
@@ -14825,7 +14825,7 @@
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B169" s="76"/>
       <c r="C169" s="0" t="s">
@@ -14840,7 +14840,7 @@
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B170" s="76"/>
       <c r="C170" s="0" t="s">
@@ -14855,7 +14855,7 @@
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="76" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="B171" s="76"/>
       <c r="C171" s="0" t="s">
@@ -14870,7 +14870,7 @@
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="76" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B172" s="76"/>
       <c r="C172" s="0" t="s">
@@ -14885,7 +14885,7 @@
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B173" s="76"/>
       <c r="C173" s="0" t="s">
@@ -14900,7 +14900,7 @@
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B174" s="76"/>
       <c r="C174" s="0" t="s">
@@ -14915,7 +14915,7 @@
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B175" s="76"/>
       <c r="C175" s="0" t="s">
@@ -14930,7 +14930,7 @@
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B176" s="76"/>
       <c r="C176" s="0" t="s">
@@ -14945,7 +14945,7 @@
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B177" s="76"/>
       <c r="C177" s="0" t="s">
@@ -14960,7 +14960,7 @@
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B178" s="76"/>
       <c r="C178" s="0" t="s">
@@ -14975,7 +14975,7 @@
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B179" s="76"/>
       <c r="C179" s="0" t="s">
@@ -14990,7 +14990,7 @@
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="76" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B180" s="76"/>
       <c r="C180" s="0" t="s">
@@ -15005,7 +15005,7 @@
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B181" s="76"/>
       <c r="C181" s="0" t="s">
@@ -15020,7 +15020,7 @@
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B182" s="76"/>
       <c r="C182" s="0" t="s">
@@ -15035,7 +15035,7 @@
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="76" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B183" s="76"/>
       <c r="C183" s="0" t="s">
@@ -15050,7 +15050,7 @@
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B184" s="76"/>
       <c r="C184" s="0" t="s">
@@ -15065,7 +15065,7 @@
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="76" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B185" s="76"/>
       <c r="C185" s="0" t="s">
@@ -15080,7 +15080,7 @@
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B186" s="76"/>
       <c r="C186" s="0" t="s">
@@ -15095,7 +15095,7 @@
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="76" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B187" s="76"/>
       <c r="C187" s="0" t="s">
@@ -15110,7 +15110,7 @@
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B188" s="76"/>
       <c r="C188" s="0" t="s">
@@ -15125,7 +15125,7 @@
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="76" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B189" s="76"/>
       <c r="C189" s="0" t="s">
@@ -15140,7 +15140,7 @@
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="76" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="B190" s="76"/>
       <c r="C190" s="0" t="s">
@@ -15155,7 +15155,7 @@
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B191" s="76"/>
       <c r="C191" s="0" t="s">
@@ -15170,7 +15170,7 @@
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="76" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B192" s="76"/>
       <c r="C192" s="0" t="s">
@@ -15185,7 +15185,7 @@
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="76" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B193" s="76"/>
       <c r="C193" s="0" t="s">
@@ -15200,7 +15200,7 @@
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B194" s="76"/>
       <c r="C194" s="0" t="s">
@@ -15215,7 +15215,7 @@
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B195" s="76"/>
       <c r="C195" s="0" t="s">
@@ -15230,7 +15230,7 @@
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B196" s="76"/>
       <c r="C196" s="0" t="s">
@@ -15245,7 +15245,7 @@
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B197" s="76"/>
       <c r="C197" s="0" t="s">
@@ -15260,7 +15260,7 @@
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="76" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B198" s="76"/>
       <c r="C198" s="0" t="s">
@@ -15275,7 +15275,7 @@
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B199" s="76"/>
       <c r="C199" s="0" t="s">
@@ -15290,7 +15290,7 @@
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B200" s="76"/>
       <c r="C200" s="0" t="s">
@@ -15305,7 +15305,7 @@
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B201" s="76"/>
       <c r="C201" s="0" t="s">
@@ -15320,7 +15320,7 @@
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="76" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B202" s="76"/>
       <c r="C202" s="0" t="s">
@@ -15335,7 +15335,7 @@
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B203" s="76"/>
       <c r="C203" s="0" t="s">
@@ -15350,7 +15350,7 @@
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="76" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="B204" s="76"/>
       <c r="C204" s="0" t="s">
@@ -15365,7 +15365,7 @@
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="76" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B205" s="76"/>
       <c r="C205" s="0" t="s">
@@ -15380,7 +15380,7 @@
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B206" s="76"/>
       <c r="C206" s="0" t="s">
@@ -15395,7 +15395,7 @@
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B207" s="76"/>
       <c r="C207" s="0" t="s">
@@ -15410,7 +15410,7 @@
     </row>
     <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B208" s="76"/>
       <c r="C208" s="0" t="s">
@@ -15425,7 +15425,7 @@
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="76" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B209" s="76"/>
       <c r="C209" s="0" t="s">
@@ -15440,7 +15440,7 @@
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="76" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B210" s="76"/>
       <c r="C210" s="0" t="s">
@@ -15455,7 +15455,7 @@
     </row>
     <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="76" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B211" s="76"/>
       <c r="C211" s="0" t="s">
@@ -15470,7 +15470,7 @@
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B212" s="76"/>
       <c r="C212" s="0" t="s">
@@ -15485,7 +15485,7 @@
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B213" s="76"/>
       <c r="C213" s="0" t="s">
@@ -15500,7 +15500,7 @@
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="76" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B214" s="76"/>
       <c r="C214" s="0" t="s">
@@ -15515,7 +15515,7 @@
     </row>
     <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B215" s="76"/>
       <c r="C215" s="0" t="s">
@@ -15530,7 +15530,7 @@
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B216" s="76"/>
       <c r="C216" s="0" t="s">
@@ -15545,7 +15545,7 @@
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B217" s="76"/>
       <c r="C217" s="0" t="s">
@@ -15560,7 +15560,7 @@
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B218" s="76"/>
       <c r="C218" s="0" t="s">
@@ -15575,7 +15575,7 @@
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="76" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="B219" s="76"/>
       <c r="C219" s="0" t="s">
@@ -15590,7 +15590,7 @@
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B220" s="76"/>
       <c r="C220" s="0" t="s">
@@ -15605,7 +15605,7 @@
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="76" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="B221" s="76"/>
       <c r="C221" s="0" t="s">
@@ -15620,7 +15620,7 @@
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B222" s="76"/>
       <c r="C222" s="0" t="s">
@@ -15635,7 +15635,7 @@
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B223" s="76"/>
       <c r="C223" s="0" t="s">
@@ -15650,7 +15650,7 @@
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B224" s="76"/>
       <c r="C224" s="0" t="s">
@@ -15665,7 +15665,7 @@
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="76" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B225" s="76"/>
       <c r="C225" s="0" t="s">
@@ -15680,7 +15680,7 @@
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="76" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B226" s="76"/>
       <c r="C226" s="0" t="s">
@@ -15695,7 +15695,7 @@
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B227" s="76"/>
       <c r="C227" s="0" t="s">
@@ -15710,7 +15710,7 @@
     </row>
     <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="76" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="B228" s="76"/>
       <c r="C228" s="0" t="s">
@@ -15725,7 +15725,7 @@
     </row>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B229" s="76"/>
       <c r="C229" s="0" t="s">
@@ -15740,7 +15740,7 @@
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B230" s="76"/>
       <c r="C230" s="0" t="s">
@@ -15755,7 +15755,7 @@
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="76" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="B231" s="76"/>
       <c r="C231" s="0" t="s">
@@ -15770,7 +15770,7 @@
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B232" s="76"/>
       <c r="C232" s="0" t="s">
@@ -15785,7 +15785,7 @@
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B233" s="76"/>
       <c r="C233" s="0" t="s">
@@ -15815,7 +15815,7 @@
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="76" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="B235" s="76"/>
       <c r="C235" s="0" t="s">
@@ -15830,7 +15830,7 @@
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="76" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B236" s="76"/>
       <c r="C236" s="0" t="s">
@@ -15845,7 +15845,7 @@
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B237" s="76"/>
       <c r="C237" s="0" t="s">
@@ -15860,7 +15860,7 @@
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B238" s="76"/>
       <c r="C238" s="0" t="s">
@@ -15875,7 +15875,7 @@
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B239" s="76"/>
       <c r="C239" s="0" t="s">
@@ -15890,7 +15890,7 @@
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="76" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B240" s="76"/>
       <c r="C240" s="0" t="s">
@@ -15905,7 +15905,7 @@
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="C241" s="0" t="s">
         <v>560</v>
@@ -15919,7 +15919,7 @@
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="C242" s="0" t="s">
         <v>562</v>
@@ -15933,7 +15933,7 @@
     </row>
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="C243" s="0" t="s">
         <v>564</v>
@@ -15947,7 +15947,7 @@
     </row>
     <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="76" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="C244" s="0" t="s">
         <v>566</v>
@@ -15961,7 +15961,7 @@
     </row>
     <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="76" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="C245" s="0" t="s">
         <v>568</v>
@@ -15975,7 +15975,7 @@
     </row>
     <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="C246" s="0" t="s">
         <v>570</v>
@@ -15989,7 +15989,7 @@
     </row>
     <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="C247" s="0" t="s">
         <v>572</v>
@@ -16003,7 +16003,7 @@
     </row>
     <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="76" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="C248" s="0" t="s">
         <v>574</v>

</xml_diff>